<commit_message>
(add test patterns for data scheme, javascript scheme)
</commit_message>
<xml_diff>
--- a/tests/testData/files/alias_without_page_id.xlsx
+++ b/tests/testData/files/alias_without_page_id.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.7-alpha.1%2Bnb</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t xml:space="preserve">/category5/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data:datascheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JavaScript Scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">javascript:alert(123);</t>
   </si>
   <si>
     <t xml:space="preserve">EndOfData</t>
@@ -146,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -170,48 +182,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="メイリオ"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF808080"/>
-      <name val="メイリオ"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006600"/>
-      <name val="メイリオ"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF996600"/>
-      <name val="メイリオ"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFCC0000"/>
-      <name val="メイリオ"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="メイリオ"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF333333"/>
       <name val="メイリオ"/>
@@ -233,54 +203,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -300,28 +228,19 @@
         <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -354,7 +273,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -378,135 +297,71 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
@@ -534,7 +389,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -561,19 +416,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="J9" activeCellId="0" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.95"/>
@@ -847,23 +702,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G22" r:id="rId1" display="data:datascheme"/>
+    <hyperlink ref="G23" r:id="rId2" display="javascript:alert(123"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>